<commit_message>
retrain model with Chris' correction on the training dataset
</commit_message>
<xml_diff>
--- a/docket_texts/Train/DT/New Topics - Classification -5.27.2018.xlsx
+++ b/docket_texts/Train/DT/New Topics - Classification -5.27.2018.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4807" uniqueCount="1246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4815" uniqueCount="1248">
   <si>
     <t xml:space="preserve">Original Docket Text</t>
   </si>
@@ -101,6 +101,9 @@
     <t xml:space="preserve">['note refile document nonecf document error .', 'note document .', '.', 'document file via .', 'file support oppose document .']</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Additional Proposed Conclusions of Law of Rohit Phansalkar. (djc) (Entered: 11/05/2001)</t>
   </si>
   <si>
@@ -113,9 +116,6 @@
     <t xml:space="preserve">Summary Judgment Filing</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">Triage</t>
   </si>
   <si>
@@ -3750,6 +3750,12 @@
   </si>
   <si>
     <t xml:space="preserve">['list']</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DECISION and ORDER: Pursuant to 28 U.S.C. § 1404, this Court hereby transfers this matter to the United States District Court for the Southern District of New York. Case transferred to District of Southern District of New York. Original file, certified copy of transfer order, and docket sheet sent. ALL FILINGS ARE TO BE MADE IN THE TRANSFER COURT, DO NOT DOCKET TO THIS CASE.. So Ordered by Judge William F. Kuntz, II on 4/17/2017. (Tavarez, Jennifer) [Transferred from New York Eastern on 4/28/2017.] (Entered: 04/19/2017)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">['decision order usc § transfer transfer original certify transfer order sheet send transfer order ii']</t>
   </si>
   <si>
     <t xml:space="preserve">Topic #</t>
@@ -3864,10 +3870,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H625"/>
+  <dimension ref="A1:H626"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J3" activeCellId="0" sqref="J3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A623" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G630" activeCellId="0" sqref="G630"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4062,28 +4068,31 @@
       <c r="F8" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>31</v>
@@ -4109,7 +4118,7 @@
         <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>31</v>
@@ -4135,7 +4144,7 @@
         <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>31</v>
@@ -4161,7 +4170,7 @@
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>31</v>
@@ -4187,7 +4196,7 @@
         <v>34</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>31</v>
@@ -4213,7 +4222,7 @@
         <v>34</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>31</v>
@@ -4239,7 +4248,7 @@
         <v>34</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>31</v>
@@ -4265,7 +4274,7 @@
         <v>48</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>31</v>
@@ -4291,7 +4300,7 @@
         <v>52</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>31</v>
@@ -4317,7 +4326,7 @@
         <v>52</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>31</v>
@@ -4340,10 +4349,10 @@
         <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>31</v>
@@ -4366,10 +4375,10 @@
         <v>10</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>31</v>
@@ -4415,10 +4424,10 @@
         <v>10</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>31</v>
@@ -4444,7 +4453,7 @@
         <v>69</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>31</v>
@@ -4470,7 +4479,7 @@
         <v>72</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>31</v>
@@ -4496,7 +4505,7 @@
         <v>76</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>31</v>
@@ -4706,7 +4715,7 @@
         <v>98</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>31</v>
@@ -4732,7 +4741,7 @@
         <v>100</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>31</v>
@@ -4758,7 +4767,7 @@
         <v>100</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>31</v>
@@ -4784,7 +4793,7 @@
         <v>100</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>31</v>
@@ -5661,7 +5670,7 @@
         <v>72</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>31</v>
@@ -5687,7 +5696,7 @@
         <v>72</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>31</v>
@@ -5874,7 +5883,7 @@
         <v>72</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>31</v>
@@ -5900,7 +5909,7 @@
         <v>72</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>31</v>
@@ -5926,7 +5935,7 @@
         <v>72</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H86" s="1" t="s">
         <v>31</v>
@@ -6064,10 +6073,10 @@
         <v>10</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>31</v>
@@ -6090,10 +6099,10 @@
         <v>10</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>31</v>
@@ -6116,10 +6125,10 @@
         <v>10</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>31</v>
@@ -6142,10 +6151,10 @@
         <v>10</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>31</v>
@@ -6191,10 +6200,10 @@
         <v>10</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H97" s="1" t="s">
         <v>31</v>
@@ -6217,10 +6226,10 @@
         <v>10</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H98" s="1" t="s">
         <v>31</v>
@@ -6243,10 +6252,10 @@
         <v>10</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H99" s="1" t="s">
         <v>31</v>
@@ -6269,10 +6278,10 @@
         <v>10</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H100" s="1" t="s">
         <v>31</v>
@@ -6295,10 +6304,10 @@
         <v>10</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H101" s="1" t="s">
         <v>31</v>
@@ -6321,10 +6330,10 @@
         <v>10</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H102" s="1" t="s">
         <v>31</v>
@@ -6347,10 +6356,10 @@
         <v>10</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>31</v>
@@ -6373,10 +6382,10 @@
         <v>10</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>31</v>
@@ -6399,10 +6408,10 @@
         <v>10</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H105" s="1" t="s">
         <v>31</v>
@@ -6428,7 +6437,7 @@
         <v>98</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>31</v>
@@ -6454,7 +6463,7 @@
         <v>98</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H107" s="1" t="s">
         <v>31</v>
@@ -6480,7 +6489,7 @@
         <v>98</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H108" s="1" t="s">
         <v>31</v>
@@ -6506,7 +6515,7 @@
         <v>229</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H109" s="1" t="s">
         <v>31</v>
@@ -6532,7 +6541,7 @@
         <v>72</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H110" s="1" t="s">
         <v>31</v>
@@ -6558,7 +6567,7 @@
         <v>234</v>
       </c>
       <c r="G111" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H111" s="1" t="s">
         <v>31</v>
@@ -6584,7 +6593,7 @@
         <v>98</v>
       </c>
       <c r="G112" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H112" s="1" t="s">
         <v>31</v>
@@ -6610,7 +6619,7 @@
         <v>240</v>
       </c>
       <c r="G113" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H113" s="1" t="s">
         <v>31</v>
@@ -6636,7 +6645,7 @@
         <v>72</v>
       </c>
       <c r="G114" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H114" s="1" t="s">
         <v>31</v>
@@ -6662,7 +6671,7 @@
         <v>52</v>
       </c>
       <c r="G115" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H115" s="1" t="s">
         <v>31</v>
@@ -6688,7 +6697,7 @@
         <v>52</v>
       </c>
       <c r="G116" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H116" s="1" t="s">
         <v>31</v>
@@ -6714,7 +6723,7 @@
         <v>52</v>
       </c>
       <c r="G117" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H117" s="1" t="s">
         <v>31</v>
@@ -6740,7 +6749,7 @@
         <v>52</v>
       </c>
       <c r="G118" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H118" s="1" t="s">
         <v>31</v>
@@ -6766,7 +6775,7 @@
         <v>52</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H119" s="1" t="s">
         <v>31</v>
@@ -6792,7 +6801,7 @@
         <v>52</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H120" s="1" t="s">
         <v>31</v>
@@ -6818,7 +6827,7 @@
         <v>52</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H121" s="1" t="s">
         <v>31</v>
@@ -6844,7 +6853,7 @@
         <v>52</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H122" s="1" t="s">
         <v>31</v>
@@ -6870,7 +6879,7 @@
         <v>52</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H123" s="1" t="s">
         <v>31</v>
@@ -6896,7 +6905,7 @@
         <v>52</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H124" s="1" t="s">
         <v>31</v>
@@ -6922,7 +6931,7 @@
         <v>52</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H125" s="1" t="s">
         <v>31</v>
@@ -6948,7 +6957,7 @@
         <v>52</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H126" s="1" t="s">
         <v>31</v>
@@ -6974,7 +6983,7 @@
         <v>52</v>
       </c>
       <c r="G127" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H127" s="1" t="s">
         <v>31</v>
@@ -7000,7 +7009,7 @@
         <v>52</v>
       </c>
       <c r="G128" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H128" s="1" t="s">
         <v>31</v>
@@ -7026,7 +7035,7 @@
         <v>52</v>
       </c>
       <c r="G129" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H129" s="1" t="s">
         <v>31</v>
@@ -7098,7 +7107,7 @@
         <v>234</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>31</v>
@@ -7124,7 +7133,7 @@
         <v>234</v>
       </c>
       <c r="G133" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H133" s="1" t="s">
         <v>31</v>
@@ -7426,7 +7435,7 @@
         <v>234</v>
       </c>
       <c r="G146" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H146" s="1" t="s">
         <v>31</v>
@@ -7452,7 +7461,7 @@
         <v>234</v>
       </c>
       <c r="G147" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H147" s="1" t="s">
         <v>31</v>
@@ -7501,7 +7510,7 @@
         <v>72</v>
       </c>
       <c r="G149" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>31</v>
@@ -7527,7 +7536,7 @@
         <v>72</v>
       </c>
       <c r="G150" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H150" s="1" t="s">
         <v>31</v>
@@ -7553,7 +7562,7 @@
         <v>72</v>
       </c>
       <c r="G151" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H151" s="1" t="s">
         <v>31</v>
@@ -7579,7 +7588,7 @@
         <v>52</v>
       </c>
       <c r="G152" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H152" s="1" t="s">
         <v>31</v>
@@ -7605,7 +7614,7 @@
         <v>52</v>
       </c>
       <c r="G153" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H153" s="1" t="s">
         <v>31</v>
@@ -7631,7 +7640,7 @@
         <v>98</v>
       </c>
       <c r="G154" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H154" s="1" t="s">
         <v>31</v>
@@ -7657,7 +7666,7 @@
         <v>98</v>
       </c>
       <c r="G155" s="2" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H155" s="2" t="s">
         <v>31</v>
@@ -7683,7 +7692,7 @@
         <v>52</v>
       </c>
       <c r="G156" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H156" s="1" t="s">
         <v>31</v>
@@ -7709,7 +7718,7 @@
         <v>52</v>
       </c>
       <c r="G157" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H157" s="1" t="s">
         <v>31</v>
@@ -7735,7 +7744,7 @@
         <v>52</v>
       </c>
       <c r="G158" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H158" s="1" t="s">
         <v>31</v>
@@ -7761,7 +7770,7 @@
         <v>52</v>
       </c>
       <c r="G159" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H159" s="1" t="s">
         <v>31</v>
@@ -7787,7 +7796,7 @@
         <v>52</v>
       </c>
       <c r="G160" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H160" s="1" t="s">
         <v>31</v>
@@ -7813,7 +7822,7 @@
         <v>52</v>
       </c>
       <c r="G161" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H161" s="1" t="s">
         <v>31</v>
@@ -7839,7 +7848,7 @@
         <v>52</v>
       </c>
       <c r="G162" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H162" s="1" t="s">
         <v>31</v>
@@ -7865,7 +7874,7 @@
         <v>52</v>
       </c>
       <c r="G163" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H163" s="1" t="s">
         <v>31</v>
@@ -7891,7 +7900,7 @@
         <v>52</v>
       </c>
       <c r="G164" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H164" s="1" t="s">
         <v>31</v>
@@ -7917,7 +7926,7 @@
         <v>52</v>
       </c>
       <c r="G165" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H165" s="1" t="s">
         <v>31</v>
@@ -7943,7 +7952,7 @@
         <v>52</v>
       </c>
       <c r="G166" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H166" s="1" t="s">
         <v>31</v>
@@ -7969,7 +7978,7 @@
         <v>52</v>
       </c>
       <c r="G167" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H167" s="1" t="s">
         <v>31</v>
@@ -7995,7 +8004,7 @@
         <v>52</v>
       </c>
       <c r="G168" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H168" s="1" t="s">
         <v>31</v>
@@ -8021,7 +8030,7 @@
         <v>52</v>
       </c>
       <c r="G169" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H169" s="1" t="s">
         <v>31</v>
@@ -8047,7 +8056,7 @@
         <v>52</v>
       </c>
       <c r="G170" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H170" s="1" t="s">
         <v>31</v>
@@ -8073,7 +8082,7 @@
         <v>52</v>
       </c>
       <c r="G171" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H171" s="1" t="s">
         <v>31</v>
@@ -8099,7 +8108,7 @@
         <v>52</v>
       </c>
       <c r="G172" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H172" s="1" t="s">
         <v>31</v>
@@ -8125,7 +8134,7 @@
         <v>52</v>
       </c>
       <c r="G173" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H173" s="1" t="s">
         <v>31</v>
@@ -8151,7 +8160,7 @@
         <v>52</v>
       </c>
       <c r="G174" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H174" s="1" t="s">
         <v>31</v>
@@ -8177,7 +8186,7 @@
         <v>52</v>
       </c>
       <c r="G175" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H175" s="1" t="s">
         <v>31</v>
@@ -8203,7 +8212,7 @@
         <v>52</v>
       </c>
       <c r="G176" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H176" s="1" t="s">
         <v>31</v>
@@ -8229,7 +8238,7 @@
         <v>52</v>
       </c>
       <c r="G177" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H177" s="1" t="s">
         <v>31</v>
@@ -8255,7 +8264,7 @@
         <v>52</v>
       </c>
       <c r="G178" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H178" s="1" t="s">
         <v>31</v>
@@ -8281,7 +8290,7 @@
         <v>52</v>
       </c>
       <c r="G179" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H179" s="1" t="s">
         <v>31</v>
@@ -8307,7 +8316,7 @@
         <v>52</v>
       </c>
       <c r="G180" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H180" s="1" t="s">
         <v>31</v>
@@ -8333,7 +8342,7 @@
         <v>52</v>
       </c>
       <c r="G181" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H181" s="1" t="s">
         <v>31</v>
@@ -8359,7 +8368,7 @@
         <v>52</v>
       </c>
       <c r="G182" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H182" s="1" t="s">
         <v>31</v>
@@ -8385,7 +8394,7 @@
         <v>52</v>
       </c>
       <c r="G183" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H183" s="1" t="s">
         <v>31</v>
@@ -8411,7 +8420,7 @@
         <v>52</v>
       </c>
       <c r="G184" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H184" s="1" t="s">
         <v>31</v>
@@ -8437,7 +8446,7 @@
         <v>52</v>
       </c>
       <c r="G185" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H185" s="1" t="s">
         <v>31</v>
@@ -8463,7 +8472,7 @@
         <v>52</v>
       </c>
       <c r="G186" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H186" s="1" t="s">
         <v>31</v>
@@ -8489,7 +8498,7 @@
         <v>52</v>
       </c>
       <c r="G187" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H187" s="1" t="s">
         <v>31</v>
@@ -8515,7 +8524,7 @@
         <v>52</v>
       </c>
       <c r="G188" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H188" s="1" t="s">
         <v>31</v>
@@ -8541,7 +8550,7 @@
         <v>52</v>
       </c>
       <c r="G189" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H189" s="1" t="s">
         <v>31</v>
@@ -8567,7 +8576,7 @@
         <v>52</v>
       </c>
       <c r="G190" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H190" s="1" t="s">
         <v>31</v>
@@ -8593,7 +8602,7 @@
         <v>52</v>
       </c>
       <c r="G191" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H191" s="1" t="s">
         <v>31</v>
@@ -8619,7 +8628,7 @@
         <v>52</v>
       </c>
       <c r="G192" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H192" s="1" t="s">
         <v>31</v>
@@ -8645,7 +8654,7 @@
         <v>52</v>
       </c>
       <c r="G193" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H193" s="1" t="s">
         <v>31</v>
@@ -8671,7 +8680,7 @@
         <v>52</v>
       </c>
       <c r="G194" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H194" s="1" t="s">
         <v>31</v>
@@ -8697,7 +8706,7 @@
         <v>52</v>
       </c>
       <c r="G195" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H195" s="1" t="s">
         <v>31</v>
@@ -8723,7 +8732,7 @@
         <v>52</v>
       </c>
       <c r="G196" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H196" s="1" t="s">
         <v>31</v>
@@ -8749,7 +8758,7 @@
         <v>52</v>
       </c>
       <c r="G197" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H197" s="1" t="s">
         <v>31</v>
@@ -8775,7 +8784,7 @@
         <v>52</v>
       </c>
       <c r="G198" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H198" s="1" t="s">
         <v>31</v>
@@ -8801,7 +8810,7 @@
         <v>52</v>
       </c>
       <c r="G199" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H199" s="1" t="s">
         <v>31</v>
@@ -8827,7 +8836,7 @@
         <v>52</v>
       </c>
       <c r="G200" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H200" s="1" t="s">
         <v>31</v>
@@ -8853,7 +8862,7 @@
         <v>52</v>
       </c>
       <c r="G201" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H201" s="1" t="s">
         <v>31</v>
@@ -8879,7 +8888,7 @@
         <v>52</v>
       </c>
       <c r="G202" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H202" s="1" t="s">
         <v>31</v>
@@ -8905,7 +8914,7 @@
         <v>52</v>
       </c>
       <c r="G203" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H203" s="1" t="s">
         <v>31</v>
@@ -8931,7 +8940,7 @@
         <v>52</v>
       </c>
       <c r="G204" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H204" s="1" t="s">
         <v>31</v>
@@ -8957,7 +8966,7 @@
         <v>52</v>
       </c>
       <c r="G205" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H205" s="1" t="s">
         <v>31</v>
@@ -8983,7 +8992,7 @@
         <v>52</v>
       </c>
       <c r="G206" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H206" s="1" t="s">
         <v>31</v>
@@ -9009,7 +9018,7 @@
         <v>52</v>
       </c>
       <c r="G207" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H207" s="1" t="s">
         <v>31</v>
@@ -9035,7 +9044,7 @@
         <v>52</v>
       </c>
       <c r="G208" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H208" s="1" t="s">
         <v>31</v>
@@ -9061,7 +9070,7 @@
         <v>52</v>
       </c>
       <c r="G209" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H209" s="1" t="s">
         <v>31</v>
@@ -9087,7 +9096,7 @@
         <v>52</v>
       </c>
       <c r="G210" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H210" s="1" t="s">
         <v>31</v>
@@ -9113,7 +9122,7 @@
         <v>52</v>
       </c>
       <c r="G211" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H211" s="1" t="s">
         <v>31</v>
@@ -9139,7 +9148,7 @@
         <v>52</v>
       </c>
       <c r="G212" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H212" s="1" t="s">
         <v>31</v>
@@ -9165,7 +9174,7 @@
         <v>52</v>
       </c>
       <c r="G213" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H213" s="1" t="s">
         <v>31</v>
@@ -9191,7 +9200,7 @@
         <v>52</v>
       </c>
       <c r="G214" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H214" s="1" t="s">
         <v>31</v>
@@ -9217,7 +9226,7 @@
         <v>52</v>
       </c>
       <c r="G215" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H215" s="1" t="s">
         <v>31</v>
@@ -9243,7 +9252,7 @@
         <v>52</v>
       </c>
       <c r="G216" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H216" s="1" t="s">
         <v>31</v>
@@ -9269,7 +9278,7 @@
         <v>52</v>
       </c>
       <c r="G217" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H217" s="1" t="s">
         <v>31</v>
@@ -9295,7 +9304,7 @@
         <v>52</v>
       </c>
       <c r="G218" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H218" s="1" t="s">
         <v>31</v>
@@ -9758,7 +9767,7 @@
         <v>72</v>
       </c>
       <c r="G238" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H238" s="1" t="s">
         <v>31</v>
@@ -9784,7 +9793,7 @@
         <v>72</v>
       </c>
       <c r="G239" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H239" s="1" t="s">
         <v>31</v>
@@ -9810,7 +9819,7 @@
         <v>72</v>
       </c>
       <c r="G240" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H240" s="1" t="s">
         <v>31</v>
@@ -9836,7 +9845,7 @@
         <v>72</v>
       </c>
       <c r="G241" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H241" s="1" t="s">
         <v>31</v>
@@ -9862,7 +9871,7 @@
         <v>72</v>
       </c>
       <c r="G242" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H242" s="1" t="s">
         <v>31</v>
@@ -9888,7 +9897,7 @@
         <v>72</v>
       </c>
       <c r="G243" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H243" s="1" t="s">
         <v>31</v>
@@ -9910,6 +9919,9 @@
       <c r="E244" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="G244" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="245" customFormat="false" ht="86.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="1" t="s">
@@ -9931,7 +9943,7 @@
         <v>72</v>
       </c>
       <c r="G245" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H245" s="1" t="s">
         <v>31</v>
@@ -9957,7 +9969,7 @@
         <v>72</v>
       </c>
       <c r="G246" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H246" s="1" t="s">
         <v>31</v>
@@ -9983,7 +9995,7 @@
         <v>72</v>
       </c>
       <c r="G247" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H247" s="1" t="s">
         <v>31</v>
@@ -10009,7 +10021,7 @@
         <v>72</v>
       </c>
       <c r="G248" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H248" s="1" t="s">
         <v>31</v>
@@ -10035,7 +10047,7 @@
         <v>72</v>
       </c>
       <c r="G249" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H249" s="1" t="s">
         <v>31</v>
@@ -10061,7 +10073,7 @@
         <v>72</v>
       </c>
       <c r="G250" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H250" s="1" t="s">
         <v>31</v>
@@ -10087,7 +10099,7 @@
         <v>72</v>
       </c>
       <c r="G251" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H251" s="1" t="s">
         <v>31</v>
@@ -10113,7 +10125,7 @@
         <v>72</v>
       </c>
       <c r="G252" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H252" s="1" t="s">
         <v>31</v>
@@ -10139,7 +10151,7 @@
         <v>72</v>
       </c>
       <c r="G253" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H253" s="1" t="s">
         <v>31</v>
@@ -10165,7 +10177,7 @@
         <v>72</v>
       </c>
       <c r="G254" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H254" s="1" t="s">
         <v>31</v>
@@ -10858,7 +10870,7 @@
         <v>229</v>
       </c>
       <c r="G284" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H284" s="1" t="s">
         <v>31</v>
@@ -10884,7 +10896,7 @@
         <v>229</v>
       </c>
       <c r="G285" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H285" s="1" t="s">
         <v>31</v>
@@ -10910,7 +10922,7 @@
         <v>229</v>
       </c>
       <c r="G286" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H286" s="1" t="s">
         <v>31</v>
@@ -10936,7 +10948,7 @@
         <v>229</v>
       </c>
       <c r="G287" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H287" s="1" t="s">
         <v>31</v>
@@ -10962,7 +10974,7 @@
         <v>229</v>
       </c>
       <c r="G288" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H288" s="1" t="s">
         <v>31</v>
@@ -10988,7 +11000,7 @@
         <v>229</v>
       </c>
       <c r="G289" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H289" s="1" t="s">
         <v>31</v>
@@ -11014,7 +11026,7 @@
         <v>229</v>
       </c>
       <c r="G290" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H290" s="1" t="s">
         <v>31</v>
@@ -11040,7 +11052,7 @@
         <v>229</v>
       </c>
       <c r="G291" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H291" s="1" t="s">
         <v>31</v>
@@ -11066,7 +11078,7 @@
         <v>229</v>
       </c>
       <c r="G292" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H292" s="1" t="s">
         <v>31</v>
@@ -11092,7 +11104,7 @@
         <v>229</v>
       </c>
       <c r="G293" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H293" s="1" t="s">
         <v>31</v>
@@ -11118,7 +11130,7 @@
         <v>229</v>
       </c>
       <c r="G294" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H294" s="1" t="s">
         <v>31</v>
@@ -11144,7 +11156,7 @@
         <v>229</v>
       </c>
       <c r="G295" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H295" s="1" t="s">
         <v>31</v>
@@ -11170,7 +11182,7 @@
         <v>229</v>
       </c>
       <c r="G296" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H296" s="1" t="s">
         <v>31</v>
@@ -11196,7 +11208,7 @@
         <v>229</v>
       </c>
       <c r="G297" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H297" s="1" t="s">
         <v>31</v>
@@ -11222,7 +11234,7 @@
         <v>229</v>
       </c>
       <c r="G298" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H298" s="1" t="s">
         <v>31</v>
@@ -11248,7 +11260,7 @@
         <v>229</v>
       </c>
       <c r="G299" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H299" s="1" t="s">
         <v>31</v>
@@ -11274,7 +11286,7 @@
         <v>229</v>
       </c>
       <c r="G300" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H300" s="1" t="s">
         <v>31</v>
@@ -11300,7 +11312,7 @@
         <v>229</v>
       </c>
       <c r="G301" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H301" s="1" t="s">
         <v>31</v>
@@ -11326,7 +11338,7 @@
         <v>229</v>
       </c>
       <c r="G302" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H302" s="1" t="s">
         <v>31</v>
@@ -11352,7 +11364,7 @@
         <v>229</v>
       </c>
       <c r="G303" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H303" s="1" t="s">
         <v>31</v>
@@ -11378,7 +11390,7 @@
         <v>229</v>
       </c>
       <c r="G304" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H304" s="1" t="s">
         <v>31</v>
@@ -11404,7 +11416,7 @@
         <v>229</v>
       </c>
       <c r="G305" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H305" s="1" t="s">
         <v>31</v>
@@ -11430,7 +11442,7 @@
         <v>229</v>
       </c>
       <c r="G306" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H306" s="1" t="s">
         <v>31</v>
@@ -11456,7 +11468,7 @@
         <v>229</v>
       </c>
       <c r="G307" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H307" s="1" t="s">
         <v>31</v>
@@ -11482,7 +11494,7 @@
         <v>229</v>
       </c>
       <c r="G308" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H308" s="1" t="s">
         <v>31</v>
@@ -11508,7 +11520,7 @@
         <v>98</v>
       </c>
       <c r="G309" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="310" customFormat="false" ht="171.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11554,7 +11566,7 @@
         <v>229</v>
       </c>
       <c r="G311" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H311" s="1" t="s">
         <v>31</v>
@@ -11580,7 +11592,7 @@
         <v>72</v>
       </c>
       <c r="G312" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H312" s="1" t="s">
         <v>31</v>
@@ -11606,7 +11618,7 @@
         <v>72</v>
       </c>
       <c r="G313" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H313" s="1" t="s">
         <v>31</v>
@@ -11632,7 +11644,7 @@
         <v>72</v>
       </c>
       <c r="G314" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H314" s="1" t="s">
         <v>31</v>
@@ -11658,7 +11670,7 @@
         <v>72</v>
       </c>
       <c r="G315" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H315" s="1" t="s">
         <v>31</v>
@@ -11684,7 +11696,7 @@
         <v>72</v>
       </c>
       <c r="G316" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H316" s="1" t="s">
         <v>31</v>
@@ -11710,7 +11722,7 @@
         <v>72</v>
       </c>
       <c r="G317" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H317" s="1" t="s">
         <v>31</v>
@@ -11736,7 +11748,7 @@
         <v>72</v>
       </c>
       <c r="G318" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H318" s="1" t="s">
         <v>31</v>
@@ -11762,7 +11774,7 @@
         <v>72</v>
       </c>
       <c r="G319" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H319" s="1" t="s">
         <v>31</v>
@@ -11788,7 +11800,7 @@
         <v>72</v>
       </c>
       <c r="G320" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H320" s="1" t="s">
         <v>31</v>
@@ -11814,7 +11826,7 @@
         <v>72</v>
       </c>
       <c r="G321" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H321" s="1" t="s">
         <v>31</v>
@@ -11840,7 +11852,7 @@
         <v>72</v>
       </c>
       <c r="G322" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H322" s="1" t="s">
         <v>31</v>
@@ -11866,7 +11878,7 @@
         <v>72</v>
       </c>
       <c r="G323" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H323" s="1" t="s">
         <v>31</v>
@@ -11892,7 +11904,7 @@
         <v>72</v>
       </c>
       <c r="G324" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H324" s="1" t="s">
         <v>31</v>
@@ -11918,7 +11930,7 @@
         <v>72</v>
       </c>
       <c r="G325" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H325" s="1" t="s">
         <v>31</v>
@@ -11944,7 +11956,7 @@
         <v>72</v>
       </c>
       <c r="G326" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H326" s="1" t="s">
         <v>31</v>
@@ -11970,7 +11982,7 @@
         <v>72</v>
       </c>
       <c r="G327" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H327" s="1" t="s">
         <v>31</v>
@@ -11996,7 +12008,7 @@
         <v>72</v>
       </c>
       <c r="G328" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H328" s="1" t="s">
         <v>31</v>
@@ -12022,7 +12034,7 @@
         <v>72</v>
       </c>
       <c r="G329" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H329" s="1" t="s">
         <v>31</v>
@@ -12048,7 +12060,7 @@
         <v>229</v>
       </c>
       <c r="G330" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H330" s="1" t="s">
         <v>31</v>
@@ -12074,7 +12086,7 @@
         <v>229</v>
       </c>
       <c r="G331" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H331" s="1" t="s">
         <v>31</v>
@@ -12100,7 +12112,7 @@
         <v>72</v>
       </c>
       <c r="G332" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H332" s="1" t="s">
         <v>31</v>
@@ -12126,7 +12138,7 @@
         <v>72</v>
       </c>
       <c r="G333" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H333" s="1" t="s">
         <v>31</v>
@@ -12152,7 +12164,7 @@
         <v>72</v>
       </c>
       <c r="G334" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H334" s="1" t="s">
         <v>31</v>
@@ -12178,7 +12190,7 @@
         <v>72</v>
       </c>
       <c r="G335" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H335" s="1" t="s">
         <v>31</v>
@@ -12204,7 +12216,7 @@
         <v>72</v>
       </c>
       <c r="G336" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H336" s="1" t="s">
         <v>31</v>
@@ -12230,7 +12242,7 @@
         <v>72</v>
       </c>
       <c r="G337" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H337" s="1" t="s">
         <v>31</v>
@@ -12256,7 +12268,7 @@
         <v>72</v>
       </c>
       <c r="G338" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H338" s="1" t="s">
         <v>31</v>
@@ -12282,7 +12294,7 @@
         <v>72</v>
       </c>
       <c r="G339" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H339" s="1" t="s">
         <v>31</v>
@@ -12308,7 +12320,7 @@
         <v>72</v>
       </c>
       <c r="G340" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H340" s="1" t="s">
         <v>31</v>
@@ -12334,7 +12346,7 @@
         <v>72</v>
       </c>
       <c r="G341" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H341" s="1" t="s">
         <v>31</v>
@@ -12360,7 +12372,7 @@
         <v>72</v>
       </c>
       <c r="G342" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H342" s="1" t="s">
         <v>31</v>
@@ -12386,7 +12398,7 @@
         <v>72</v>
       </c>
       <c r="G343" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H343" s="1" t="s">
         <v>31</v>
@@ -12412,7 +12424,7 @@
         <v>72</v>
       </c>
       <c r="G344" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H344" s="1" t="s">
         <v>31</v>
@@ -12438,7 +12450,7 @@
         <v>72</v>
       </c>
       <c r="G345" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H345" s="1" t="s">
         <v>31</v>
@@ -12464,7 +12476,7 @@
         <v>72</v>
       </c>
       <c r="G346" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H346" s="1" t="s">
         <v>31</v>
@@ -12490,7 +12502,7 @@
         <v>72</v>
       </c>
       <c r="G347" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H347" s="1" t="s">
         <v>31</v>
@@ -12516,7 +12528,7 @@
         <v>72</v>
       </c>
       <c r="G348" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H348" s="1" t="s">
         <v>31</v>
@@ -12542,7 +12554,7 @@
         <v>72</v>
       </c>
       <c r="G349" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H349" s="1" t="s">
         <v>31</v>
@@ -12568,7 +12580,7 @@
         <v>72</v>
       </c>
       <c r="G350" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H350" s="1" t="s">
         <v>31</v>
@@ -12594,7 +12606,7 @@
         <v>72</v>
       </c>
       <c r="G351" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H351" s="1" t="s">
         <v>31</v>
@@ -12620,7 +12632,7 @@
         <v>72</v>
       </c>
       <c r="G352" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H352" s="1" t="s">
         <v>31</v>
@@ -12646,7 +12658,7 @@
         <v>72</v>
       </c>
       <c r="G353" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H353" s="1" t="s">
         <v>31</v>
@@ -12672,7 +12684,7 @@
         <v>72</v>
       </c>
       <c r="G354" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H354" s="1" t="s">
         <v>31</v>
@@ -12698,7 +12710,7 @@
         <v>72</v>
       </c>
       <c r="G355" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H355" s="1" t="s">
         <v>31</v>
@@ -12724,7 +12736,7 @@
         <v>72</v>
       </c>
       <c r="G356" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H356" s="1" t="s">
         <v>31</v>
@@ -12750,7 +12762,7 @@
         <v>72</v>
       </c>
       <c r="G357" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H357" s="1" t="s">
         <v>31</v>
@@ -12776,7 +12788,7 @@
         <v>72</v>
       </c>
       <c r="G358" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H358" s="1" t="s">
         <v>31</v>
@@ -12802,7 +12814,7 @@
         <v>72</v>
       </c>
       <c r="G359" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H359" s="1" t="s">
         <v>31</v>
@@ -12828,7 +12840,7 @@
         <v>72</v>
       </c>
       <c r="G360" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H360" s="1" t="s">
         <v>31</v>
@@ -12854,7 +12866,7 @@
         <v>72</v>
       </c>
       <c r="G361" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H361" s="1" t="s">
         <v>31</v>
@@ -12880,7 +12892,7 @@
         <v>72</v>
       </c>
       <c r="G362" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H362" s="1" t="s">
         <v>31</v>
@@ -12906,7 +12918,7 @@
         <v>72</v>
       </c>
       <c r="G363" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H363" s="1" t="s">
         <v>31</v>
@@ -12932,7 +12944,7 @@
         <v>72</v>
       </c>
       <c r="G364" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H364" s="1" t="s">
         <v>31</v>
@@ -12958,7 +12970,7 @@
         <v>229</v>
       </c>
       <c r="G365" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H365" s="1" t="s">
         <v>31</v>
@@ -13027,10 +13039,10 @@
         <v>10</v>
       </c>
       <c r="F368" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G368" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H368" s="1" t="s">
         <v>31</v>
@@ -13053,10 +13065,10 @@
         <v>10</v>
       </c>
       <c r="F369" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G369" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H369" s="1" t="s">
         <v>31</v>
@@ -13079,10 +13091,10 @@
         <v>10</v>
       </c>
       <c r="F370" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G370" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H370" s="1" t="s">
         <v>31</v>
@@ -13105,10 +13117,10 @@
         <v>10</v>
       </c>
       <c r="F371" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G371" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H371" s="1" t="s">
         <v>31</v>
@@ -13131,10 +13143,10 @@
         <v>10</v>
       </c>
       <c r="F372" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G372" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H372" s="1" t="s">
         <v>31</v>
@@ -13157,10 +13169,10 @@
         <v>10</v>
       </c>
       <c r="F373" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G373" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H373" s="1" t="s">
         <v>31</v>
@@ -13183,10 +13195,10 @@
         <v>10</v>
       </c>
       <c r="F374" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G374" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H374" s="1" t="s">
         <v>31</v>
@@ -13209,10 +13221,10 @@
         <v>10</v>
       </c>
       <c r="F375" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G375" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H375" s="1" t="s">
         <v>31</v>
@@ -13235,10 +13247,10 @@
         <v>10</v>
       </c>
       <c r="F376" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G376" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H376" s="1" t="s">
         <v>31</v>
@@ -13264,7 +13276,7 @@
         <v>98</v>
       </c>
       <c r="G377" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H377" s="1" t="s">
         <v>31</v>
@@ -13290,7 +13302,7 @@
         <v>98</v>
       </c>
       <c r="G378" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H378" s="1" t="s">
         <v>31</v>
@@ -13316,7 +13328,7 @@
         <v>234</v>
       </c>
       <c r="G379" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H379" s="1" t="s">
         <v>31</v>
@@ -13342,7 +13354,7 @@
         <v>234</v>
       </c>
       <c r="G380" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H380" s="1" t="s">
         <v>31</v>
@@ -13368,7 +13380,7 @@
         <v>234</v>
       </c>
       <c r="G381" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H381" s="1" t="s">
         <v>31</v>
@@ -13394,7 +13406,7 @@
         <v>234</v>
       </c>
       <c r="G382" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H382" s="1" t="s">
         <v>31</v>
@@ -13420,7 +13432,7 @@
         <v>98</v>
       </c>
       <c r="G383" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H383" s="1" t="s">
         <v>31</v>
@@ -13446,7 +13458,7 @@
         <v>98</v>
       </c>
       <c r="G384" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H384" s="1" t="s">
         <v>31</v>
@@ -13472,7 +13484,7 @@
         <v>72</v>
       </c>
       <c r="G385" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H385" s="1" t="s">
         <v>31</v>
@@ -13498,7 +13510,7 @@
         <v>72</v>
       </c>
       <c r="G386" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H386" s="1" t="s">
         <v>31</v>
@@ -13521,10 +13533,10 @@
         <v>10</v>
       </c>
       <c r="F387" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G387" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H387" s="1" t="s">
         <v>31</v>
@@ -13550,7 +13562,7 @@
         <v>72</v>
       </c>
       <c r="G388" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H388" s="1" t="s">
         <v>31</v>
@@ -13576,7 +13588,7 @@
         <v>72</v>
       </c>
       <c r="G389" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H389" s="1" t="s">
         <v>31</v>
@@ -13602,7 +13614,7 @@
         <v>234</v>
       </c>
       <c r="G390" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H390" s="1" t="s">
         <v>31</v>
@@ -13628,7 +13640,7 @@
         <v>234</v>
       </c>
       <c r="G391" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H391" s="1" t="s">
         <v>31</v>
@@ -13654,7 +13666,7 @@
         <v>234</v>
       </c>
       <c r="G392" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H392" s="1" t="s">
         <v>31</v>
@@ -13680,7 +13692,7 @@
         <v>234</v>
       </c>
       <c r="G393" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H393" s="1" t="s">
         <v>31</v>
@@ -13706,7 +13718,7 @@
         <v>234</v>
       </c>
       <c r="G394" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H394" s="1" t="s">
         <v>31</v>
@@ -13729,10 +13741,10 @@
         <v>10</v>
       </c>
       <c r="F395" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G395" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H395" s="1" t="s">
         <v>31</v>
@@ -13755,10 +13767,10 @@
         <v>10</v>
       </c>
       <c r="F396" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G396" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H396" s="1" t="s">
         <v>31</v>
@@ -13781,10 +13793,10 @@
         <v>10</v>
       </c>
       <c r="F397" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G397" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H397" s="1" t="s">
         <v>31</v>
@@ -13807,10 +13819,10 @@
         <v>10</v>
       </c>
       <c r="F398" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G398" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H398" s="1" t="s">
         <v>31</v>
@@ -13833,10 +13845,10 @@
         <v>10</v>
       </c>
       <c r="F399" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G399" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H399" s="1" t="s">
         <v>31</v>
@@ -13859,10 +13871,10 @@
         <v>10</v>
       </c>
       <c r="F400" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G400" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H400" s="1" t="s">
         <v>31</v>
@@ -13885,10 +13897,10 @@
         <v>10</v>
       </c>
       <c r="F401" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G401" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H401" s="1" t="s">
         <v>31</v>
@@ -13911,10 +13923,10 @@
         <v>10</v>
       </c>
       <c r="F402" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G402" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H402" s="1" t="s">
         <v>31</v>
@@ -13937,10 +13949,10 @@
         <v>10</v>
       </c>
       <c r="F403" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G403" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H403" s="1" t="s">
         <v>31</v>
@@ -13963,10 +13975,10 @@
         <v>10</v>
       </c>
       <c r="F404" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G404" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H404" s="1" t="s">
         <v>31</v>
@@ -13989,10 +14001,10 @@
         <v>10</v>
       </c>
       <c r="F405" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G405" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H405" s="1" t="s">
         <v>31</v>
@@ -14015,10 +14027,10 @@
         <v>10</v>
       </c>
       <c r="F406" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G406" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H406" s="1" t="s">
         <v>31</v>
@@ -14041,10 +14053,10 @@
         <v>10</v>
       </c>
       <c r="F407" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G407" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H407" s="1" t="s">
         <v>31</v>
@@ -14067,10 +14079,10 @@
         <v>10</v>
       </c>
       <c r="F408" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G408" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H408" s="1" t="s">
         <v>31</v>
@@ -14093,10 +14105,10 @@
         <v>10</v>
       </c>
       <c r="F409" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G409" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H409" s="1" t="s">
         <v>31</v>
@@ -14119,10 +14131,10 @@
         <v>10</v>
       </c>
       <c r="F410" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G410" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H410" s="1" t="s">
         <v>31</v>
@@ -14145,10 +14157,10 @@
         <v>10</v>
       </c>
       <c r="F411" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G411" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H411" s="1" t="s">
         <v>31</v>
@@ -14171,10 +14183,10 @@
         <v>10</v>
       </c>
       <c r="F412" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G412" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H412" s="1" t="s">
         <v>31</v>
@@ -14197,10 +14209,10 @@
         <v>10</v>
       </c>
       <c r="F413" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G413" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H413" s="1" t="s">
         <v>31</v>
@@ -14223,10 +14235,10 @@
         <v>10</v>
       </c>
       <c r="F414" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G414" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H414" s="1" t="s">
         <v>31</v>
@@ -14249,10 +14261,10 @@
         <v>10</v>
       </c>
       <c r="F415" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G415" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H415" s="1" t="s">
         <v>31</v>
@@ -14275,10 +14287,10 @@
         <v>10</v>
       </c>
       <c r="F416" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G416" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H416" s="1" t="s">
         <v>31</v>
@@ -14301,10 +14313,10 @@
         <v>10</v>
       </c>
       <c r="F417" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G417" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H417" s="1" t="s">
         <v>31</v>
@@ -14327,10 +14339,10 @@
         <v>10</v>
       </c>
       <c r="F418" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G418" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H418" s="1" t="s">
         <v>31</v>
@@ -14353,10 +14365,10 @@
         <v>10</v>
       </c>
       <c r="F419" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G419" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H419" s="1" t="s">
         <v>31</v>
@@ -14379,10 +14391,10 @@
         <v>10</v>
       </c>
       <c r="F420" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G420" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H420" s="1" t="s">
         <v>31</v>
@@ -14405,10 +14417,10 @@
         <v>10</v>
       </c>
       <c r="F421" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G421" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H421" s="1" t="s">
         <v>31</v>
@@ -14431,10 +14443,10 @@
         <v>10</v>
       </c>
       <c r="F422" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G422" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H422" s="1" t="s">
         <v>31</v>
@@ -14457,10 +14469,10 @@
         <v>10</v>
       </c>
       <c r="F423" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G423" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H423" s="1" t="s">
         <v>31</v>
@@ -14483,10 +14495,10 @@
         <v>10</v>
       </c>
       <c r="F424" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G424" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H424" s="1" t="s">
         <v>31</v>
@@ -14509,10 +14521,10 @@
         <v>10</v>
       </c>
       <c r="F425" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G425" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H425" s="1" t="s">
         <v>31</v>
@@ -14535,10 +14547,10 @@
         <v>10</v>
       </c>
       <c r="F426" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G426" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H426" s="1" t="s">
         <v>31</v>
@@ -14561,10 +14573,10 @@
         <v>10</v>
       </c>
       <c r="F427" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G427" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H427" s="1" t="s">
         <v>31</v>
@@ -14587,10 +14599,10 @@
         <v>10</v>
       </c>
       <c r="F428" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G428" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H428" s="1" t="s">
         <v>31</v>
@@ -14613,10 +14625,10 @@
         <v>10</v>
       </c>
       <c r="F429" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G429" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H429" s="1" t="s">
         <v>31</v>
@@ -14639,10 +14651,10 @@
         <v>10</v>
       </c>
       <c r="F430" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G430" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H430" s="1" t="s">
         <v>31</v>
@@ -15588,7 +15600,7 @@
         <v>72</v>
       </c>
       <c r="G471" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H471" s="1" t="s">
         <v>31</v>
@@ -15614,7 +15626,7 @@
         <v>72</v>
       </c>
       <c r="G472" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H472" s="1" t="s">
         <v>31</v>
@@ -15640,7 +15652,7 @@
         <v>72</v>
       </c>
       <c r="G473" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H473" s="1" t="s">
         <v>31</v>
@@ -15666,7 +15678,7 @@
         <v>72</v>
       </c>
       <c r="G474" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H474" s="1" t="s">
         <v>31</v>
@@ -15692,7 +15704,7 @@
         <v>72</v>
       </c>
       <c r="G475" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H475" s="1" t="s">
         <v>31</v>
@@ -15718,7 +15730,7 @@
         <v>72</v>
       </c>
       <c r="G476" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H476" s="1" t="s">
         <v>31</v>
@@ -15744,7 +15756,7 @@
         <v>72</v>
       </c>
       <c r="G477" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H477" s="1" t="s">
         <v>31</v>
@@ -15770,7 +15782,7 @@
         <v>72</v>
       </c>
       <c r="G478" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H478" s="1" t="s">
         <v>31</v>
@@ -15796,7 +15808,7 @@
         <v>72</v>
       </c>
       <c r="G479" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H479" s="1" t="s">
         <v>31</v>
@@ -16650,7 +16662,7 @@
         <v>72</v>
       </c>
       <c r="G516" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H516" s="1" t="s">
         <v>31</v>
@@ -16676,7 +16688,7 @@
         <v>72</v>
       </c>
       <c r="G517" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H517" s="1" t="s">
         <v>31</v>
@@ -16702,7 +16714,7 @@
         <v>72</v>
       </c>
       <c r="G518" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H518" s="1" t="s">
         <v>31</v>
@@ -16728,7 +16740,7 @@
         <v>72</v>
       </c>
       <c r="G519" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H519" s="1" t="s">
         <v>31</v>
@@ -16754,7 +16766,7 @@
         <v>72</v>
       </c>
       <c r="G520" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H520" s="1" t="s">
         <v>31</v>
@@ -16780,7 +16792,7 @@
         <v>72</v>
       </c>
       <c r="G521" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H521" s="1" t="s">
         <v>31</v>
@@ -16806,7 +16818,7 @@
         <v>72</v>
       </c>
       <c r="G522" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H522" s="1" t="s">
         <v>31</v>
@@ -16832,7 +16844,7 @@
         <v>72</v>
       </c>
       <c r="G523" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H523" s="1" t="s">
         <v>31</v>
@@ -16858,7 +16870,7 @@
         <v>72</v>
       </c>
       <c r="G524" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H524" s="1" t="s">
         <v>31</v>
@@ -16884,7 +16896,7 @@
         <v>72</v>
       </c>
       <c r="G525" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H525" s="1" t="s">
         <v>31</v>
@@ -16910,7 +16922,7 @@
         <v>72</v>
       </c>
       <c r="G526" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H526" s="1" t="s">
         <v>31</v>
@@ -16936,7 +16948,7 @@
         <v>72</v>
       </c>
       <c r="G527" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H527" s="1" t="s">
         <v>31</v>
@@ -16962,7 +16974,7 @@
         <v>1078</v>
       </c>
       <c r="G528" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H528" s="1" t="s">
         <v>31</v>
@@ -16988,7 +17000,7 @@
         <v>1078</v>
       </c>
       <c r="G529" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H529" s="1" t="s">
         <v>31</v>
@@ -17011,10 +17023,10 @@
         <v>10</v>
       </c>
       <c r="F530" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G530" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H530" s="1" t="s">
         <v>31</v>
@@ -17040,7 +17052,7 @@
         <v>52</v>
       </c>
       <c r="G531" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H531" s="1" t="s">
         <v>31</v>
@@ -17066,7 +17078,7 @@
         <v>52</v>
       </c>
       <c r="G532" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H532" s="1" t="s">
         <v>31</v>
@@ -17092,7 +17104,7 @@
         <v>52</v>
       </c>
       <c r="G533" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H533" s="1" t="s">
         <v>31</v>
@@ -17118,7 +17130,7 @@
         <v>52</v>
       </c>
       <c r="G534" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H534" s="1" t="s">
         <v>31</v>
@@ -17144,7 +17156,7 @@
         <v>52</v>
       </c>
       <c r="G535" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H535" s="1" t="s">
         <v>31</v>
@@ -17170,7 +17182,7 @@
         <v>52</v>
       </c>
       <c r="G536" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H536" s="1" t="s">
         <v>31</v>
@@ -17196,7 +17208,7 @@
         <v>52</v>
       </c>
       <c r="G537" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H537" s="1" t="s">
         <v>31</v>
@@ -17222,7 +17234,7 @@
         <v>52</v>
       </c>
       <c r="G538" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H538" s="1" t="s">
         <v>31</v>
@@ -17248,7 +17260,7 @@
         <v>52</v>
       </c>
       <c r="G539" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H539" s="1" t="s">
         <v>31</v>
@@ -17274,7 +17286,7 @@
         <v>52</v>
       </c>
       <c r="G540" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H540" s="1" t="s">
         <v>31</v>
@@ -17300,7 +17312,7 @@
         <v>52</v>
       </c>
       <c r="G541" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H541" s="1" t="s">
         <v>31</v>
@@ -17326,7 +17338,7 @@
         <v>52</v>
       </c>
       <c r="G542" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H542" s="1" t="s">
         <v>31</v>
@@ -17352,7 +17364,7 @@
         <v>52</v>
       </c>
       <c r="G543" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H543" s="1" t="s">
         <v>31</v>
@@ -17378,7 +17390,7 @@
         <v>72</v>
       </c>
       <c r="G544" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H544" s="1" t="s">
         <v>31</v>
@@ -17404,7 +17416,7 @@
         <v>72</v>
       </c>
       <c r="G545" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H545" s="1" t="s">
         <v>31</v>
@@ -17430,7 +17442,7 @@
         <v>72</v>
       </c>
       <c r="G546" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H546" s="1" t="s">
         <v>31</v>
@@ -17456,7 +17468,7 @@
         <v>234</v>
       </c>
       <c r="G547" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H547" s="1" t="s">
         <v>31</v>
@@ -17482,7 +17494,7 @@
         <v>234</v>
       </c>
       <c r="G548" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H548" s="1" t="s">
         <v>31</v>
@@ -17531,7 +17543,7 @@
         <v>100</v>
       </c>
       <c r="G550" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H550" s="1" t="s">
         <v>31</v>
@@ -17554,10 +17566,10 @@
         <v>10</v>
       </c>
       <c r="F551" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G551" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H551" s="1" t="s">
         <v>31</v>
@@ -17583,7 +17595,7 @@
         <v>72</v>
       </c>
       <c r="G552" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H552" s="1" t="s">
         <v>31</v>
@@ -17655,7 +17667,7 @@
         <v>234</v>
       </c>
       <c r="G555" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H555" s="1" t="s">
         <v>31</v>
@@ -17819,7 +17831,7 @@
         <v>1150</v>
       </c>
       <c r="G562" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H562" s="1" t="s">
         <v>31</v>
@@ -17845,7 +17857,7 @@
         <v>1150</v>
       </c>
       <c r="G563" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H563" s="1" t="s">
         <v>31</v>
@@ -17871,7 +17883,7 @@
         <v>1150</v>
       </c>
       <c r="G564" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H564" s="1" t="s">
         <v>31</v>
@@ -17897,7 +17909,7 @@
         <v>1150</v>
       </c>
       <c r="G565" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H565" s="1" t="s">
         <v>31</v>
@@ -17923,7 +17935,7 @@
         <v>1150</v>
       </c>
       <c r="G566" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H566" s="1" t="s">
         <v>31</v>
@@ -17949,7 +17961,7 @@
         <v>1150</v>
       </c>
       <c r="G567" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H567" s="1" t="s">
         <v>31</v>
@@ -17975,7 +17987,7 @@
         <v>1150</v>
       </c>
       <c r="G568" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H568" s="1" t="s">
         <v>31</v>
@@ -18001,7 +18013,7 @@
         <v>1150</v>
       </c>
       <c r="G569" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H569" s="1" t="s">
         <v>31</v>
@@ -18027,7 +18039,7 @@
         <v>1150</v>
       </c>
       <c r="G570" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H570" s="1" t="s">
         <v>31</v>
@@ -18053,7 +18065,7 @@
         <v>1150</v>
       </c>
       <c r="G571" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H571" s="1" t="s">
         <v>31</v>
@@ -18079,7 +18091,7 @@
         <v>1150</v>
       </c>
       <c r="G572" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H572" s="1" t="s">
         <v>31</v>
@@ -18105,7 +18117,7 @@
         <v>1150</v>
       </c>
       <c r="G573" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H573" s="1" t="s">
         <v>31</v>
@@ -18131,7 +18143,7 @@
         <v>1150</v>
       </c>
       <c r="G574" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H574" s="1" t="s">
         <v>31</v>
@@ -18157,7 +18169,7 @@
         <v>1150</v>
       </c>
       <c r="G575" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H575" s="1" t="s">
         <v>31</v>
@@ -18183,7 +18195,7 @@
         <v>1150</v>
       </c>
       <c r="G576" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H576" s="1" t="s">
         <v>31</v>
@@ -18209,7 +18221,7 @@
         <v>1150</v>
       </c>
       <c r="G577" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H577" s="1" t="s">
         <v>31</v>
@@ -18235,7 +18247,7 @@
         <v>1150</v>
       </c>
       <c r="G578" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H578" s="1" t="s">
         <v>31</v>
@@ -18261,7 +18273,7 @@
         <v>1150</v>
       </c>
       <c r="G579" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H579" s="1" t="s">
         <v>31</v>
@@ -18287,7 +18299,7 @@
         <v>1150</v>
       </c>
       <c r="G580" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H580" s="1" t="s">
         <v>31</v>
@@ -18313,7 +18325,7 @@
         <v>1150</v>
       </c>
       <c r="G581" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H581" s="1" t="s">
         <v>31</v>
@@ -18339,7 +18351,7 @@
         <v>1150</v>
       </c>
       <c r="G582" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H582" s="1" t="s">
         <v>31</v>
@@ -18365,7 +18377,7 @@
         <v>1150</v>
       </c>
       <c r="G583" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H583" s="1" t="s">
         <v>31</v>
@@ -18391,7 +18403,7 @@
         <v>1150</v>
       </c>
       <c r="G584" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H584" s="1" t="s">
         <v>31</v>
@@ -18417,7 +18429,7 @@
         <v>1150</v>
       </c>
       <c r="G585" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H585" s="1" t="s">
         <v>31</v>
@@ -18443,7 +18455,7 @@
         <v>1150</v>
       </c>
       <c r="G586" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H586" s="1" t="s">
         <v>31</v>
@@ -18469,7 +18481,7 @@
         <v>1150</v>
       </c>
       <c r="G587" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H587" s="1" t="s">
         <v>31</v>
@@ -18495,7 +18507,7 @@
         <v>1150</v>
       </c>
       <c r="G588" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H588" s="1" t="s">
         <v>31</v>
@@ -18521,7 +18533,7 @@
         <v>1150</v>
       </c>
       <c r="G589" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H589" s="1" t="s">
         <v>31</v>
@@ -18547,7 +18559,7 @@
         <v>1150</v>
       </c>
       <c r="G590" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H590" s="1" t="s">
         <v>31</v>
@@ -18573,7 +18585,7 @@
         <v>1150</v>
       </c>
       <c r="G591" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H591" s="1" t="s">
         <v>31</v>
@@ -18599,7 +18611,7 @@
         <v>1150</v>
       </c>
       <c r="G592" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H592" s="1" t="s">
         <v>31</v>
@@ -18625,7 +18637,7 @@
         <v>1150</v>
       </c>
       <c r="G593" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H593" s="1" t="s">
         <v>31</v>
@@ -18651,7 +18663,7 @@
         <v>1150</v>
       </c>
       <c r="G594" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H594" s="1" t="s">
         <v>31</v>
@@ -18677,7 +18689,7 @@
         <v>1150</v>
       </c>
       <c r="G595" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H595" s="1" t="s">
         <v>31</v>
@@ -18703,7 +18715,7 @@
         <v>1150</v>
       </c>
       <c r="G596" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H596" s="1" t="s">
         <v>31</v>
@@ -18729,7 +18741,7 @@
         <v>1150</v>
       </c>
       <c r="G597" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H597" s="1" t="s">
         <v>31</v>
@@ -18755,7 +18767,7 @@
         <v>1150</v>
       </c>
       <c r="G598" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H598" s="1" t="s">
         <v>31</v>
@@ -18781,7 +18793,7 @@
         <v>1150</v>
       </c>
       <c r="G599" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H599" s="1" t="s">
         <v>31</v>
@@ -18807,7 +18819,7 @@
         <v>1150</v>
       </c>
       <c r="G600" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H600" s="1" t="s">
         <v>31</v>
@@ -18833,7 +18845,7 @@
         <v>1150</v>
       </c>
       <c r="G601" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H601" s="1" t="s">
         <v>31</v>
@@ -18859,7 +18871,7 @@
         <v>1150</v>
       </c>
       <c r="G602" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H602" s="1" t="s">
         <v>31</v>
@@ -18885,7 +18897,7 @@
         <v>1150</v>
       </c>
       <c r="G603" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H603" s="1" t="s">
         <v>31</v>
@@ -18911,7 +18923,7 @@
         <v>1150</v>
       </c>
       <c r="G604" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H604" s="1" t="s">
         <v>31</v>
@@ -18937,7 +18949,7 @@
         <v>1150</v>
       </c>
       <c r="G605" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H605" s="1" t="s">
         <v>31</v>
@@ -18963,7 +18975,7 @@
         <v>1150</v>
       </c>
       <c r="G606" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H606" s="1" t="s">
         <v>31</v>
@@ -18989,7 +19001,7 @@
         <v>1150</v>
       </c>
       <c r="G607" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H607" s="1" t="s">
         <v>31</v>
@@ -19015,7 +19027,7 @@
         <v>1150</v>
       </c>
       <c r="G608" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H608" s="1" t="s">
         <v>31</v>
@@ -19386,7 +19398,7 @@
         <v>229</v>
       </c>
       <c r="G624" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H624" s="1" t="s">
         <v>31</v>
@@ -19412,10 +19424,30 @@
         <v>98</v>
       </c>
       <c r="G625" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H625" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="626" s="2" customFormat="true" ht="185.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A626" s="2" t="s">
+        <v>1243</v>
+      </c>
+      <c r="B626" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C626" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D626" s="2" t="s">
+        <v>1244</v>
+      </c>
+      <c r="E626" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G626" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -19449,16 +19481,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19469,7 +19501,7 @@
         <v>34</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>31</v>
@@ -19483,7 +19515,7 @@
         <v>69</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>31</v>
@@ -19497,7 +19529,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>31</v>
@@ -19511,7 +19543,7 @@
         <v>72</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D5" s="0" t="s">
         <v>31</v>
@@ -19525,7 +19557,7 @@
         <v>76</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>31</v>
@@ -19539,7 +19571,7 @@
         <v>48</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
         <v>31</v>
@@ -19553,7 +19585,7 @@
         <v>1078</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>31</v>
@@ -19567,7 +19599,7 @@
         <v>234</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>31</v>
@@ -19581,7 +19613,7 @@
         <v>52</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>31</v>
@@ -19595,7 +19627,7 @@
         <v>229</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>31</v>
@@ -19606,10 +19638,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>31</v>
@@ -19645,7 +19677,7 @@
         <v>98</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D15" s="0" t="s">
         <v>31</v>

</xml_diff>